<commit_message>
tạo hồ sơ pv đợt 2
</commit_message>
<xml_diff>
--- a/hồ sơ_đợt 1/tổng hợp_cv.xlsx
+++ b/hồ sơ_đợt 1/tổng hợp_cv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="198">
   <si>
     <t>Họ Tên</t>
   </si>
@@ -633,6 +633,12 @@
   </si>
   <si>
     <t>Chuyên viên/ KTV Hạ tầng CNTT ?</t>
+  </si>
+  <si>
+    <t>canhnt88@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nghiatt1119@gmail.com </t>
   </si>
 </sst>
 </file>
@@ -850,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1083,6 +1089,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1369,8 +1378,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1534,7 @@
         <v>9636.0963699999993</v>
       </c>
       <c r="O3" s="82" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
       <c r="P3" s="91" t="s">
         <v>152</v>
@@ -1671,7 +1680,7 @@
       <c r="N6" s="86">
         <v>372553817</v>
       </c>
-      <c r="O6" s="66" t="s">
+      <c r="O6" s="98" t="s">
         <v>17</v>
       </c>
       <c r="P6" s="86" t="s">
@@ -1679,110 +1688,117 @@
       </c>
       <c r="S6" s="93"/>
     </row>
-    <row r="7" spans="1:20" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
-        <v>191</v>
+    <row r="7" spans="1:20" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="85" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="85" t="s">
         <v>189</v>
       </c>
       <c r="C7" s="86" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="D7" s="56" t="s">
         <v>125</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
+      <c r="G7" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>177</v>
+      </c>
       <c r="I7" s="56" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="J7" s="56" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="K7" s="88" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="M7" s="87">
-        <v>1994</v>
-      </c>
-      <c r="N7" s="85">
-        <v>366167337</v>
-      </c>
-      <c r="O7" s="83" t="s">
-        <v>85</v>
+        <v>139</v>
+      </c>
+      <c r="M7" s="86">
+        <v>1990</v>
+      </c>
+      <c r="N7" s="86">
+        <v>967467622</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="P7" s="86" t="s">
-        <v>86</v>
-      </c>
-      <c r="S7" s="93"/>
-    </row>
-    <row r="8" spans="1:20" s="92" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+    </row>
+    <row r="8" spans="1:20" s="86" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B8" s="85" t="s">
         <v>189</v>
       </c>
       <c r="C8" s="86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D8" s="56" t="s">
         <v>125</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="56" t="s">
         <v>161</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="J8" s="56" t="s">
         <v>174</v>
       </c>
       <c r="K8" s="88" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="M8" s="86">
         <v>1990</v>
       </c>
-      <c r="N8" s="86">
-        <v>967467622</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>25</v>
+      <c r="N8" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="72" t="s">
+        <v>197</v>
       </c>
       <c r="P8" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q8" s="86"/>
-      <c r="R8" s="86"/>
-    </row>
-    <row r="9" spans="1:20" s="86" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="85" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="C9" s="86" t="s">
-        <v>194</v>
+        <v>14</v>
+      </c>
+      <c r="R8" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="S8" s="93"/>
+    </row>
+    <row r="9" spans="1:20" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>50</v>
       </c>
       <c r="D9" s="56" t="s">
         <v>125</v>
@@ -1791,286 +1807,278 @@
         <v>132</v>
       </c>
       <c r="F9" s="56"/>
-      <c r="G9" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="H9" s="56" t="s">
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="K9" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="59">
+        <v>912740868</v>
+      </c>
+      <c r="O9" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="P9" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q9" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="R9" s="56"/>
+      <c r="T9" s="61"/>
+    </row>
+    <row r="10" spans="1:20" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="I9" s="56" t="s">
-        <v>165</v>
-      </c>
-      <c r="J9" s="56" t="s">
-        <v>174</v>
-      </c>
-      <c r="K9" s="88" t="s">
-        <v>155</v>
-      </c>
-      <c r="L9" s="57" t="s">
-        <v>157</v>
-      </c>
-      <c r="M9" s="86">
-        <v>1990</v>
-      </c>
-      <c r="N9" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="O9" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="R9" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="S9" s="93"/>
-    </row>
-    <row r="10" spans="1:20" s="95" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="94" t="s">
-        <v>192</v>
-      </c>
-      <c r="C10" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J10" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="K10" s="96" t="s">
-        <v>138</v>
-      </c>
-      <c r="L10" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="M10" s="95">
-        <v>1990</v>
-      </c>
-      <c r="N10" s="95">
-        <v>974698017</v>
-      </c>
-      <c r="O10" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="95" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q10" s="95" t="s">
-        <v>74</v>
-      </c>
-      <c r="S10" s="97"/>
-    </row>
-    <row r="11" spans="1:20" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="L10" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10" s="87">
+        <v>1994</v>
+      </c>
+      <c r="N10" s="85">
+        <v>366167337</v>
+      </c>
+      <c r="O10" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="P10" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="S10" s="93"/>
+    </row>
+    <row r="11" spans="1:20" s="95" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B11" s="94" t="s">
         <v>192</v>
       </c>
       <c r="C11" s="95" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D11" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>178</v>
-      </c>
+      <c r="E11" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="56" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="J11" s="56" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="K11" s="96" t="s">
         <v>138</v>
       </c>
-      <c r="L11" s="57" t="s">
-        <v>139</v>
+      <c r="L11" s="56" t="s">
+        <v>142</v>
       </c>
       <c r="M11" s="95">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="N11" s="95">
-        <v>364289198</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="P11" s="95"/>
-      <c r="Q11" s="95"/>
-      <c r="R11" s="95" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>974698017</v>
+      </c>
+      <c r="O11" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11" s="95" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q11" s="95" t="s">
+        <v>74</v>
+      </c>
+      <c r="S11" s="97"/>
+    </row>
+    <row r="12" spans="1:20" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="94" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B12" s="94" t="s">
         <v>192</v>
       </c>
       <c r="C12" s="95" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="J12" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="K12" s="96" t="s">
+        <v>138</v>
+      </c>
+      <c r="L12" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="M12" s="95">
+        <v>1995</v>
+      </c>
+      <c r="N12" s="95">
+        <v>364289198</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" s="95"/>
+      <c r="Q12" s="95"/>
+      <c r="R12" s="95" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="56" t="s">
+      <c r="D13" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="56" t="s">
         <v>133</v>
-      </c>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="J12" s="56" t="s">
-        <v>128</v>
-      </c>
-      <c r="K12" s="96" t="s">
-        <v>167</v>
-      </c>
-      <c r="L12" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="M12" s="95">
-        <v>1996</v>
-      </c>
-      <c r="N12" s="95">
-        <v>394693918</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="95" t="s">
-        <v>77</v>
-      </c>
-      <c r="R12" s="95"/>
-    </row>
-    <row r="13" spans="1:20" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>137</v>
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
       <c r="H13" s="56"/>
       <c r="I13" s="56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J13" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="K13" s="57" t="s">
-        <v>138</v>
+      <c r="K13" s="96" t="s">
+        <v>167</v>
       </c>
       <c r="L13" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="M13" s="56">
-        <v>1984</v>
-      </c>
-      <c r="N13" s="56">
-        <v>936471473</v>
+        <v>141</v>
+      </c>
+      <c r="M13" s="95">
+        <v>1996</v>
+      </c>
+      <c r="N13" s="95">
+        <v>394693918</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="P13" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-    </row>
-    <row r="14" spans="1:20" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="P13" s="95" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="95" t="s">
+        <v>77</v>
+      </c>
+      <c r="R13" s="95"/>
+    </row>
+    <row r="14" spans="1:20" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>190</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D14" s="56" t="s">
         <v>125</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F14" s="56"/>
-      <c r="G14" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="H14" s="56" t="s">
-        <v>132</v>
-      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="56" t="s">
         <v>131</v>
       </c>
       <c r="J14" s="56" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="K14" s="57" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="L14" s="57" t="s">
-        <v>182</v>
-      </c>
-      <c r="M14" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="N14" s="56" t="s">
-        <v>109</v>
+        <v>139</v>
+      </c>
+      <c r="M14" s="56">
+        <v>1984</v>
+      </c>
+      <c r="N14" s="56">
+        <v>936471473</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="P14" s="56" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="Q14" s="56"/>
       <c r="R14" s="56"/>
     </row>
-    <row r="15" spans="1:20" s="55" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="B15" s="53" t="s">
         <v>190</v>
@@ -2082,14 +2090,14 @@
         <v>125</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F15" s="56"/>
       <c r="G15" s="56" t="s">
         <v>161</v>
       </c>
       <c r="H15" s="56" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
       <c r="I15" s="56" t="s">
         <v>131</v>
@@ -2104,70 +2112,71 @@
         <v>182</v>
       </c>
       <c r="M15" s="56" t="s">
-        <v>171</v>
+        <v>110</v>
       </c>
       <c r="N15" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="O15" s="66" t="s">
-        <v>172</v>
+        <v>109</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="P15" s="56" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="Q15" s="56"/>
       <c r="R15" s="56"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="23"/>
-    </row>
-    <row r="16" spans="1:20" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
-        <v>188</v>
+    </row>
+    <row r="16" spans="1:20" s="55" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
+        <v>169</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>190</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D16" s="56" t="s">
         <v>125</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>179</v>
+      </c>
       <c r="I16" s="56" t="s">
         <v>131</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="K16" s="57" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="L16" s="57" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="M16" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="N16" s="59">
-        <v>912740868</v>
-      </c>
-      <c r="O16" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="P16" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q16" s="60" t="s">
-        <v>97</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="N16" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="O16" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="P16" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q16" s="56"/>
       <c r="R16" s="56"/>
-      <c r="T16" s="61"/>
+      <c r="S16" s="73"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="1:20" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
@@ -2922,12 +2931,14 @@
     <hyperlink ref="N17" r:id="rId3" display="tel:0397113271"/>
     <hyperlink ref="O31" r:id="rId4"/>
     <hyperlink ref="O20" r:id="rId5" display="mailto:xtho.lthuong@gmail.com"/>
-    <hyperlink ref="O11" r:id="rId6"/>
+    <hyperlink ref="O12" r:id="rId6"/>
     <hyperlink ref="O5" r:id="rId7"/>
     <hyperlink ref="O28" r:id="rId8"/>
+    <hyperlink ref="O8" r:id="rId9"/>
+    <hyperlink ref="O6" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
kêt thúc đợt 3
</commit_message>
<xml_diff>
--- a/hồ sơ_đợt 1/tổng hợp_cv.xlsx
+++ b/hồ sơ_đợt 1/tổng hợp_cv.xlsx
@@ -1378,20 +1378,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" style="53" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="23" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="26" style="23" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="53" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="23" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="23" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="23" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="23" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="23" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="23" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="23" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="23" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="23" customWidth="1"/>

</xml_diff>